<commit_message>
feat(parsers): add sheet name support for v3 BOM parsing
- Extended Board model with sheet_name attribute to capture Excel sheet source

- Updated _v3_bom_parser functions to pass and assign sheet_name when parsing boards

- Modified unit tests to verify sheet_name is correctly populated and asserted

- Refreshed Version3BomSample.xlsx to include sheet name validation in tests
</commit_message>
<xml_diff>
--- a/tests/parsers/test_data/Version3BomSample.xlsx
+++ b/tests/parsers/test_data/Version3BomSample.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\ElectricalBomAnalyser\tests\parsers\test_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\BomBuddy\tests\parsers\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A4357AF-D705-4618-85FA-2F87961A036B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{095A4587-6273-4EF3-9F03-B869635041FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15150" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="844" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" tabRatio="844" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="PCBA BOM Template" sheetId="12" r:id="rId1"/>
+    <sheet name="POWER PCBA" sheetId="12" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'PCBA BOM Template'!$K$5:$N$15</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'PCBA BOM Template'!$A$1:$N$15</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'POWER PCBA'!$K$5:$N$15</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'POWER PCBA'!$A$1:$N$15</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -872,7 +872,7 @@
   <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="55" workbookViewId="0">
-      <selection activeCell="N11" sqref="A1:N11"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1133,7 +1133,7 @@
         <v>0.7</v>
       </c>
       <c r="N7" s="19">
-        <f t="shared" ref="N7:N13" si="0">M7*K7</f>
+        <f t="shared" ref="N7:N9" si="0">M7*K7</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>